<commit_message>
feat: add multi-institute support
</commit_message>
<xml_diff>
--- a/api/public/template/TEMPLATE-IMPOR-SISWA.xlsx
+++ b/api/public/template/TEMPLATE-IMPOR-SISWA.xlsx
@@ -32,19 +32,40 @@
     <t>nama</t>
   </si>
   <si>
+    <t>no_induk</t>
+  </si>
+  <si>
+    <t>jenis_kelamin</t>
+  </si>
+  <si>
+    <t>nisn</t>
+  </si>
+  <si>
     <t>tempat_lahir</t>
   </si>
   <si>
     <t>tgl_lahir</t>
   </si>
   <si>
-    <t>no_induk</t>
-  </si>
-  <si>
-    <t>nisn</t>
-  </si>
-  <si>
-    <t>jenis_kelamin</t>
+    <t>alamat</t>
+  </si>
+  <si>
+    <t>rt</t>
+  </si>
+  <si>
+    <t>rw</t>
+  </si>
+  <si>
+    <t>kelurahan</t>
+  </si>
+  <si>
+    <t>kecamatan</t>
+  </si>
+  <si>
+    <t>kab_kota</t>
+  </si>
+  <si>
+    <t>provinsi</t>
   </si>
   <si>
     <t>nama_ayah</t>
@@ -57,27 +78,6 @@
   </si>
   <si>
     <t>pekerjaan_ibu</t>
-  </si>
-  <si>
-    <t>alamat</t>
-  </si>
-  <si>
-    <t>rt</t>
-  </si>
-  <si>
-    <t>rw</t>
-  </si>
-  <si>
-    <t>kelurahan</t>
-  </si>
-  <si>
-    <t>kecamatan</t>
-  </si>
-  <si>
-    <t>kab_kota</t>
-  </si>
-  <si>
-    <t>provinsi</t>
   </si>
 </sst>
 </file>
@@ -1246,28 +1246,28 @@
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="37.4444444444444" customWidth="1"/>
-    <col min="2" max="2" width="13.4444444444444" customWidth="1"/>
-    <col min="3" max="3" width="11.1111111111111" customWidth="1"/>
-    <col min="4" max="4" width="10.6666666666667" customWidth="1"/>
-    <col min="5" max="5" width="11.8888888888889" customWidth="1"/>
-    <col min="6" max="6" width="13" customWidth="1"/>
-    <col min="7" max="7" width="23.8888888888889" customWidth="1"/>
-    <col min="8" max="8" width="16.6666666666667" customWidth="1"/>
-    <col min="9" max="9" width="23.4444444444444" customWidth="1"/>
-    <col min="10" max="10" width="16.6666666666667" customWidth="1"/>
-    <col min="11" max="11" width="42.6666666666667" customWidth="1"/>
-    <col min="12" max="12" width="3.66666666666667" customWidth="1"/>
-    <col min="13" max="13" width="3.77777777777778" customWidth="1"/>
-    <col min="14" max="14" width="16.4444444444444" customWidth="1"/>
-    <col min="15" max="15" width="11.4444444444444" customWidth="1"/>
-    <col min="16" max="16" width="9.22222222222222" customWidth="1"/>
-    <col min="17" max="17" width="10.7777777777778" customWidth="1"/>
+    <col min="2" max="2" width="10.6666666666667" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="4" max="4" width="11.8888888888889" customWidth="1"/>
+    <col min="5" max="5" width="13.4444444444444" customWidth="1"/>
+    <col min="6" max="6" width="11.1111111111111" customWidth="1"/>
+    <col min="7" max="7" width="42.6666666666667" customWidth="1"/>
+    <col min="8" max="8" width="3.66666666666667" customWidth="1"/>
+    <col min="9" max="9" width="3.77777777777778" customWidth="1"/>
+    <col min="10" max="10" width="16.4444444444444" customWidth="1"/>
+    <col min="11" max="11" width="11.4444444444444" customWidth="1"/>
+    <col min="12" max="12" width="9.22222222222222" customWidth="1"/>
+    <col min="13" max="13" width="10.7777777777778" customWidth="1"/>
+    <col min="14" max="14" width="23.8888888888889" customWidth="1"/>
+    <col min="15" max="15" width="16.6666666666667" customWidth="1"/>
+    <col min="16" max="16" width="23.4444444444444" customWidth="1"/>
+    <col min="17" max="17" width="16.6666666666667" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17">

</xml_diff>

<commit_message>
return student import template to the beginning version
</commit_message>
<xml_diff>
--- a/api/public/template/TEMPLATE-IMPOR-SISWA.xlsx
+++ b/api/public/template/TEMPLATE-IMPOR-SISWA.xlsx
@@ -4,12 +4,14 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22188" windowHeight="9000" activeTab="1"/>
+    <workbookView windowWidth="22188" windowHeight="9000"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Petunjuk" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$Q$1</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>nama</t>
   </si>
@@ -79,18 +81,6 @@
   </si>
   <si>
     <t>pekerjaan_ibu</t>
-  </si>
-  <si>
-    <t>Jenis Kelamin cukup isi dengan L atau P</t>
-  </si>
-  <si>
-    <t>Tanggal lahir harus dalam format YYYY-MM-DD</t>
-  </si>
-  <si>
-    <t>No induk diisi dengan 9 karakter</t>
-  </si>
-  <si>
-    <t>NISN diisi dengan 10 karakter</t>
   </si>
 </sst>
 </file>
@@ -1261,12 +1251,12 @@
   <sheetPr/>
   <dimension ref="A1:Q1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="J11" sqref="J11"/>
+      <selection pane="bottomRight" activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
@@ -1281,7 +1271,7 @@
     <col min="8" max="8" width="3.66666666666667" customWidth="1"/>
     <col min="9" max="9" width="3.77777777777778" customWidth="1"/>
     <col min="10" max="10" width="16.4444444444444" customWidth="1"/>
-    <col min="11" max="11" width="11.4444444444444" customWidth="1"/>
+    <col min="11" max="11" width="18" customWidth="1"/>
     <col min="12" max="12" width="9.22222222222222" customWidth="1"/>
     <col min="13" max="13" width="10.7777777777778" customWidth="1"/>
     <col min="14" max="14" width="23.8888888888889" customWidth="1"/>
@@ -1344,71 +1334,10 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="u7h/ASpq8mmDQNXu+CMopGv+jRhYeq6o7yjRi98Ikq2Ug8y1/0hZiss/OR7MvBMfUnZ1LSPyezsHbO0Rar3gWg==" saltValue="62WbyP3ukdcTEJy1ZZkuGQ==" spinCount="100000" sheet="1" objects="1"/>
-  <protectedRanges>
-    <protectedRange sqref="A2:Q12000" name="data siswa"/>
-  </protectedRanges>
+  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:Q1" etc:filterBottomFollowUsedRange="0">
+    <extLst/>
+  </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr>
-    <tabColor rgb="FFFFFF00"/>
-  </sheetPr>
-  <dimension ref="A1:A4"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="3"/>
-  <cols>
-    <col min="1" max="1" width="55.2222222222222" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1">
-      <c r="A4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<allowEditUser xmlns="https://web.wps.cn/et/2018/main" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main" hasInvisiblePropRange="0">
-  <rangeList sheetStid="1" master="" otherUserPermission="visible">
-    <arrUserId title="data siswa" rangeCreator="" othersAccessPermission="edit"/>
-  </rangeList>
-  <rangeList sheetStid="2" master="" otherUserPermission="visible"/>
-</allowEditUser>
-</file>
-
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5A5607D9-04D2-4DE1-AC0E-A7772F01BC71}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="https://web.wps.cn/et/2018/main"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>